<commit_message>
Added T-Tests and results
</commit_message>
<xml_diff>
--- a/20kResults.xlsx
+++ b/20kResults.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_3A70\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{60B8C79E-726E-4E64-BFF4-4E43C7600970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9DD693B8-B2AD-4760-9AFD-B9CCFFC5840E}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{60B8C79E-726E-4E64-BFF4-4E43C7600970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31413B9D-0158-40C3-A7CD-EE50AAE8264C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="27600" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,9 +984,9 @@
       <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>85.316336149999998</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>88.574129339999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>85.316336149999998</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>87.488198280000006</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>87.110483650000006</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>87.582623960000006</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>86.449480059999999</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>88.29084039</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.252122159999999</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>86.779981849999999</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>88.149195910000003</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87.440979479999996</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>86.827194689999999</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>86.355054379999999</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>0.67017465799999998</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>85.410767789999994</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>85.269123320000006</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>88.12240869</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>86.355054379999999</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>0.60833490499999998</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>85.269123320000006</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87.252122159999999</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>0.52945908200000003</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>85.221904519999995</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>85.269123320000006</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>85.930120939999995</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>-2.0212288639999998</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85.309398169999994</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>2.5170767E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>85.309398169999994</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>1.68595446</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>86.537551879999995</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>5.0341534E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S22" t="s">
         <v>30</v>
       </c>
@@ -1435,17 +1435,17 @@
         <v>2.0243941639999998</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="V26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P27" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O28" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O29" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>87.657324369999998</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O30" t="s">
         <v>12</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>0.45058325999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O31" t="s">
         <v>14</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O32" t="s">
         <v>22</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>0.56037895900000001</v>
       </c>
     </row>
-    <row r="33" spans="15:23">
+    <row r="33" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O33" t="s">
         <v>17</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="15:23">
+    <row r="34" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O34" t="s">
         <v>25</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="15:23">
+    <row r="35" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O35" t="s">
         <v>26</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>-6.5825454959999998</v>
       </c>
     </row>
-    <row r="36" spans="15:23">
+    <row r="36" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O36" t="s">
         <v>28</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>4.53893E-8</v>
       </c>
     </row>
-    <row r="37" spans="15:23">
+    <row r="37" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O37" t="s">
         <v>29</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>1.68595446</v>
       </c>
     </row>
-    <row r="38" spans="15:23">
+    <row r="38" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O38" t="s">
         <v>30</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>9.0778700000000005E-8</v>
       </c>
     </row>
-    <row r="39" spans="15:23">
+    <row r="39" spans="15:23" x14ac:dyDescent="0.25">
       <c r="V39" t="s">
         <v>30</v>
       </c>

</xml_diff>